<commit_message>
LITE-23303: Add translation sync command
</commit_message>
<xml_diff>
--- a/tests/fixtures/translation.xlsx
+++ b/tests/fixtures/translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosherrero/projects/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F81117C-5A33-0543-9447-5A45A822308A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B3AEF5-EF00-634A-A2C0-AAFA82060348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="39360" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-39060" yWindow="-1860" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
   <si>
     <t xml:space="preserve">This is an export of attributes for a translation.
 Please check the "General" tab for more details about this translation.
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>TRN-8100-3865-4869</t>
-  </si>
-  <si>
-    <t>Translation Owner</t>
   </si>
   <si>
     <t>VA-063-000</t>
@@ -260,20 +257,32 @@
     <t>This is a translation for a test product</t>
   </si>
   <si>
-    <t>original value</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Translation Owner ID</t>
+  </si>
+  <si>
+    <t>Translation Owner Name</t>
+  </si>
+  <si>
+    <t>Vendor account 00</t>
+  </si>
+  <si>
+    <t>Persian (TRN-1079-0833-9890)</t>
+  </si>
+  <si>
+    <t>editor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +301,12 @@
     </font>
     <font>
       <sz val="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -321,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -338,15 +353,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -692,63 +708,71 @@
     </row>
     <row r="2" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="54" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="54" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="27" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{79101B26-3B07-2648-8597-A8952DEDD6CF}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{79101B26-3B07-2648-8597-A8952DEDD6CF}">
       <formula1>"Enabled,Disabled"</formula1>
     </dataValidation>
   </dataValidations>
@@ -758,11 +782,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -773,401 +797,494 @@
     <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B23" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B25" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B27" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B30" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>72</v>
+      <c r="C31" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="F31" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix translation xlsx fixtures
</commit_message>
<xml_diff>
--- a/tests/fixtures/translation.xlsx
+++ b/tests/fixtures/translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpaul00/cloud-blue-github/connect-cli/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosherrero/projects/connect-cli/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EDF3D2-A892-DE4C-ABED-40BAC76548AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B3AEF5-EF00-634A-A2C0-AAFA82060348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-39060" yWindow="-1860" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="76">
   <si>
     <t xml:space="preserve">This is an export of attributes for a translation.
 Please check the "General" tab for more details about this translation.
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>TRN-8100-3865-4869</t>
-  </si>
-  <si>
-    <t>Translation Owner</t>
   </si>
   <si>
     <t>VA-063-000</t>
@@ -266,14 +263,26 @@
     <t>-</t>
   </si>
   <si>
+    <t>Translation Owner ID</t>
+  </si>
+  <si>
+    <t>Translation Owner Name</t>
+  </si>
+  <si>
+    <t>Vendor account 00</t>
+  </si>
+  <si>
     <t>Persian (TRN-1079-0833-9890)</t>
+  </si>
+  <si>
+    <t>editor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,16 +293,20 @@
     <font>
       <sz val="20"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="20"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -323,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -340,15 +353,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -694,63 +708,71 @@
     </row>
     <row r="2" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="54" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="54" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="27" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="27" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{79101B26-3B07-2648-8597-A8952DEDD6CF}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{79101B26-3B07-2648-8597-A8952DEDD6CF}">
       <formula1>"Enabled,Disabled"</formula1>
     </dataValidation>
   </dataValidations>
@@ -760,11 +782,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -775,401 +797,494 @@
     <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B23" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B25" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B27" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B30" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>71</v>
+      <c r="C31" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="F31" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>